<commit_message>
Tabla actualizada en documentación
</commit_message>
<xml_diff>
--- a/Documentación/TABLA-empalme-remarcador.xlsx
+++ b/Documentación/TABLA-empalme-remarcador.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proy\remarcadores\programa\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="20115" windowHeight="7740"/>
+    <workbookView xWindow="120" yWindow="108" windowWidth="20112" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -297,7 +302,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,6 +312,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -521,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -691,6 +702,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -701,6 +727,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -749,7 +778,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -784,7 +813,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -996,21 +1025,21 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A24" sqref="A24:G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="28.5546875" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>78</v>
       </c>
@@ -1033,7 +1062,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1052,7 +1081,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -1073,7 +1102,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
@@ -1094,7 +1123,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>0</v>
       </c>
@@ -1115,7 +1144,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -1136,7 +1165,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>0</v>
       </c>
@@ -1157,7 +1186,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>0</v>
       </c>
@@ -1178,7 +1207,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>0</v>
       </c>
@@ -1199,7 +1228,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +1249,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>0</v>
       </c>
@@ -1241,7 +1270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>0</v>
       </c>
@@ -1262,7 +1291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>0</v>
       </c>
@@ -1283,7 +1312,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>0</v>
       </c>
@@ -1304,7 +1333,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>0</v>
       </c>
@@ -1325,7 +1354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>0</v>
       </c>
@@ -1346,7 +1375,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>0</v>
       </c>
@@ -1367,7 +1396,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>0</v>
       </c>
@@ -1388,7 +1417,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="48" t="s">
         <v>0</v>
       </c>
@@ -1409,7 +1438,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>0</v>
       </c>
@@ -1430,7 +1459,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>0</v>
       </c>
@@ -1451,7 +1480,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>38</v>
       </c>
@@ -1472,7 +1501,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>38</v>
       </c>
@@ -1493,28 +1522,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="21" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="60">
         <v>31</v>
       </c>
-      <c r="D24" s="23" t="s">
+      <c r="D24" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="25"/>
-      <c r="G24" s="24" t="s">
+      <c r="F24" s="62"/>
+      <c r="G24" s="60" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>38</v>
       </c>
@@ -1535,7 +1564,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>38</v>
       </c>
@@ -1556,7 +1585,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>38</v>
       </c>
@@ -1577,7 +1606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>38</v>
       </c>
@@ -1598,7 +1627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>38</v>
       </c>
@@ -1619,7 +1648,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>38</v>
       </c>
@@ -1640,7 +1669,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="42" t="s">
         <v>38</v>
       </c>
@@ -1661,7 +1690,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="48" t="s">
         <v>38</v>
       </c>
@@ -1682,7 +1711,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>38</v>
       </c>
@@ -1703,7 +1732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>38</v>
       </c>
@@ -1724,7 +1753,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>38</v>
       </c>
@@ -1743,7 +1772,7 @@
       <c r="F35" s="32"/>
       <c r="G35" s="10"/>
     </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
         <v>38</v>
       </c>
@@ -1762,7 +1791,7 @@
       <c r="F36" s="35"/>
       <c r="G36" s="14"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>38</v>
       </c>
@@ -1783,7 +1812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>38</v>
       </c>
@@ -1804,7 +1833,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>38</v>
       </c>
@@ -1825,7 +1854,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>38</v>
       </c>
@@ -1846,7 +1875,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>38</v>
       </c>
@@ -1867,7 +1896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
         <v>38</v>
       </c>
@@ -1888,7 +1917,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>38</v>
       </c>
@@ -1909,7 +1938,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
         <v>38</v>
       </c>
@@ -1930,7 +1959,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="12" t="s">
         <v>38</v>
       </c>
@@ -1951,7 +1980,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="36" t="s">
         <v>38</v>
       </c>
@@ -1979,7 +2008,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1991,7 +2020,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>